<commit_message>
Ajout modification de la quantité
</commit_message>
<xml_diff>
--- a/Backlog2.xlsx
+++ b/Backlog2.xlsx
@@ -351,7 +351,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -361,6 +361,7 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutre" xfId="2" builtinId="28"/>
@@ -1867,7 +1868,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,46 +1917,46 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1975,30 +1976,40 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E11" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E12" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="122" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>